<commit_message>
EPBDS-5606 Enhance indexed conditions in DT: relativity operations index completeness.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680" activeTab="1"/>
@@ -181,8 +181,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,7 +465,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -478,9 +478,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -518,7 +518,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -552,6 +552,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -586,9 +587,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -761,14 +763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
@@ -776,94 +778,94 @@
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>-5</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
@@ -871,7 +873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
@@ -879,7 +881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
@@ -887,46 +889,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="E31" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="E32" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>0</v>
       </c>
@@ -937,13 +939,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="6">
         <v>1</v>
       </c>
@@ -962,14 +964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:K38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
@@ -979,7 +981,7 @@
     <col min="11" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>18</v>
       </c>
@@ -993,7 +995,7 @@
       </c>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1027,7 +1029,7 @@
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1131,7 @@
       </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:11">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1153,7 +1155,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1181,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>1</v>
       </c>
@@ -1193,7 +1195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -1207,160 +1209,152 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="1">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="F22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="F22" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="F23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="G28" s="8">
+      <c r="C28" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="15" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="2:7" ht="32.25" customHeight="1">
-      <c r="B32" s="18" t="s">
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="15" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
-    </row>
-    <row r="35" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B35" s="18" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="15" t="s">
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
-    </row>
-    <row r="38" spans="2:4" ht="69.75" customHeight="1">
-      <c r="B38" s="18" t="s">
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="2:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add test for cast aliases.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Alias Datatype Declaration" sheetId="1" r:id="rId1"/>
     <sheet name="Alias Datatype Usage Proper" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>CA</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>CA,AR</t>
+  </si>
+  <si>
+    <t>return x;</t>
+  </si>
+  <si>
+    <t>Method String method4(State2 x)</t>
+  </si>
+  <si>
+    <t>Method State2 method5(String x)</t>
   </si>
 </sst>
 </file>
@@ -766,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1181,7 +1190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>1</v>
       </c>
@@ -1195,7 +1204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -1209,13 +1218,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F21" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>22</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1239,7 +1248,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1279,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>1</v>
       </c>
@@ -1290,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>1</v>
       </c>
@@ -1298,42 +1307,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="16"/>
       <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F31" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="17"/>
     </row>
-    <row r="37" spans="2:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="18" t="s">
         <v>26</v>
       </c>
@@ -1341,7 +1370,9 @@
       <c r="D37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
@@ -1355,6 +1386,8 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-5593 Auto casts in OpenL fix.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/datatype/AliasDatatypeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="21855" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Alias Datatype Declaration" sheetId="1" r:id="rId1"/>
@@ -451,9 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,6 +468,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,18 +991,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="C3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="J3" s="14" t="s">
+      <c r="G3" s="20"/>
+      <c r="J3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="14"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1131,14 +1131,14 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="F13" s="14" t="s">
+      <c r="C13" s="20"/>
+      <c r="F13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -1308,69 +1308,70 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="F30" s="15" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="F30" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="16"/>
     </row>
     <row r="31" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="F31" s="18" t="s">
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
+      <c r="F31" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="17"/>
-      <c r="F33" s="15" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="F33" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="17"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="F34" s="18" t="s">
+      <c r="C34" s="18"/>
+      <c r="D34" s="19"/>
+      <c r="F34" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
     </row>
     <row r="37" spans="2:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F31:H31"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="J3:K3"/>
@@ -1387,7 +1388,6 @@
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>